<commit_message>
Atualizando o arquivo historico_taxas.xlsx
</commit_message>
<xml_diff>
--- a/historico_taxas.xlsx
+++ b/historico_taxas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,20 +469,20 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46249</v>
+        <v>45792</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-04-04 13:05:55</t>
+          <t>2025-04-04 13:06:11</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46522</v>
+        <v>46249</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -495,20 +495,20 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46980</v>
+        <v>46249</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-04-04 13:05:55</t>
+          <t>2025-04-04 13:06:11</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>47253</v>
+        <v>46522</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -521,20 +521,20 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>47710</v>
+        <v>46522</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-04-04 13:05:55</t>
+          <t>2025-04-04 13:06:11</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>48441</v>
+        <v>46980</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -547,20 +547,20 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>48714</v>
+        <v>46980</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-04-04 13:05:55</t>
+          <t>2025-04-04 13:06:11</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>49444</v>
+        <v>47253</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -573,20 +573,20 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>51363</v>
+        <v>47253</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-04-04 13:05:55</t>
+          <t>2025-04-04 13:06:11</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>53097</v>
+        <v>47710</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -599,20 +599,20 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>55015</v>
+        <v>47710</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-04-04 13:05:55</t>
+          <t>2025-04-04 13:06:11</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>56749</v>
+        <v>48441</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -625,14 +625,196 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
+        <v>48441</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:06:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>48714</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:06:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>48714</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:05:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>49444</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:05:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>49444</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:06:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>51363</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:06:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>51363</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:05:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>53097</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:06:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>53097</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:05:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>55015</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:06:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>55015</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:05:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>56749</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:06:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>56749</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:05:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
         <v>58668</v>
       </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2025-04-04 13:05:55</t>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:05:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>58668</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-04-04 13:06:11</t>
         </is>
       </c>
     </row>

</xml_diff>